<commit_message>
pertemuan 10 - praktikum 1
</commit_message>
<xml_diff>
--- a/public/template_level.xlsx
+++ b/public/template_level.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9536E4E6-AD98-4BBD-B828-A8D2C9162DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0A27AE-443B-4401-84B9-300C87124F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>No</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Duty Manager Store</t>
+  </si>
+  <si>
+    <t>DRTU</t>
+  </si>
+  <si>
+    <t>Direktur Keuangan</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,6 +439,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>